<commit_message>
Added VAS safety transistor
</commit_message>
<xml_diff>
--- a/OpAmp-top.xlsx
+++ b/OpAmp-top.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="63">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">C_0805_HandSoldering</t>
   </si>
   <si>
-    <t xml:space="preserve">top</t>
+    <t xml:space="preserve">  top</t>
   </si>
   <si>
     <t xml:space="preserve">C2</t>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">Q16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q17</t>
   </si>
   <si>
     <t xml:space="preserve">R1</t>
@@ -301,20 +304,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="9.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,20 +854,20 @@
       <c r="A24" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>37</v>
+      <c r="B24" s="0" t="n">
+        <v>5401</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>69.05</v>
+        <v>72.136</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>-59.05</v>
+        <v>-60.96</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>10</v>
@@ -871,22 +875,22 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="D25" s="0" t="n">
-        <v>65.1</v>
+        <v>67.95</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>-79.175</v>
+        <v>-59.02</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>10</v>
@@ -894,22 +898,22 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>37</v>
-      </c>
       <c r="C26" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>63.925</v>
+        <v>65.1</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>-59.075</v>
+        <v>-79.175</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>10</v>
@@ -920,19 +924,19 @@
         <v>42</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>-78.95</v>
+        <v>-59</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>10</v>
@@ -943,16 +947,16 @@
         <v>43</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>79.5</v>
+        <v>75</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>-61.45</v>
+        <v>-78.95</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>270</v>
@@ -963,22 +967,22 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="C29" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>72.6</v>
+        <v>79.5</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>-68.55</v>
+        <v>-61.45</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>10</v>
@@ -986,22 +990,22 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="C30" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>72.5</v>
+        <v>72.6</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>-70.825</v>
+        <v>-68.55</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>10</v>
@@ -1012,19 +1016,19 @@
         <v>48</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>76.25</v>
+        <v>72.5</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>-61.55</v>
+        <v>-70.825</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>10</v>
@@ -1032,22 +1036,22 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="C32" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>82.15</v>
+        <v>76.25</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>-66.75</v>
+        <v>-61.55</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>10</v>
@@ -1055,19 +1059,19 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="C33" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>82.5</v>
+        <v>82.15</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>-69.8</v>
+        <v>-66.75</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>0</v>
@@ -1078,22 +1082,22 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="C34" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>91.675</v>
+        <v>82.5</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>-75.7</v>
+        <v>-69.8</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>10</v>
@@ -1101,22 +1105,22 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="C35" s="0" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>85.4</v>
+        <v>91.675</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>-80.2</v>
+        <v>-75.7</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>10</v>
@@ -1124,22 +1128,22 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="D36" s="0" t="n">
-        <v>82.57</v>
+        <v>85.4</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>-80.19</v>
+        <v>-80.2</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="G36" s="0" t="s">
         <v>10</v>
@@ -1150,19 +1154,19 @@
         <v>59</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>67.5</v>
+        <v>82.57</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>-70.15</v>
+        <v>-80.19</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>10</v>
@@ -1173,13 +1177,13 @@
         <v>60</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>62.35</v>
+        <v>67.5</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>-70.15</v>
@@ -1194,6 +1198,29 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>61</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>62.35</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>-70.15</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>